<commit_message>
Open Account Test Added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>firstName</t>
   </si>
@@ -49,7 +49,13 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>USD</t>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -414,27 +420,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Multiple parametrization added to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>firstName</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>Dollar</t>
+  </si>
+  <si>
+    <t>Hermoine Granger</t>
+  </si>
+  <si>
+    <t>Ron Weasly</t>
+  </si>
+  <si>
+    <t>Albus Dumbledore</t>
   </si>
 </sst>
 </file>
@@ -91,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,8 +416,8 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>950125</v>
+      <c r="C2" s="1">
+        <v>95125</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -415,20 +425,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,7 +456,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -454,7 +465,41 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Run mode parameterization in Excel added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -12,15 +12,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccount" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomer" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccount" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -65,6 +66,27 @@
   </si>
   <si>
     <t>Albus Dumbledore</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>AddCustomer</t>
+  </si>
+  <si>
+    <t>OpenAccount</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>loginAsManager</t>
   </si>
 </sst>
 </file>
@@ -383,9 +405,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -429,7 +502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Set up run modes for Test Data (For each test) Hashtable introduced as DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -408,7 +408,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -504,10 +504,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -526,8 +526,11 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -537,8 +540,11 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -548,8 +554,11 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -559,8 +568,11 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -569,6 +581,9 @@
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>